<commit_message>
Music player with tempo, octaves, and different note types
</commit_message>
<xml_diff>
--- a/Presentations/Gantt Chart.xlsx
+++ b/Presentations/Gantt Chart.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\OneDrive - UNSW\Documents\2017 Semester 2\COMP3601 - Desgin Project A\Git Repositry\Presentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="97" documentId="C685E72BA27742A5988848DE9270A9F692B2FFBC" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21" xr10:uidLastSave="{C19839EE-7A0A-4BEC-B8E6-76B26FC5D67A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19368" windowHeight="10572"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19368" windowHeight="10572" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Week 2</t>
   </si>
@@ -59,9 +60,6 @@
     <t>Week 12</t>
   </si>
   <si>
-    <t>Week 13</t>
-  </si>
-  <si>
     <t>Web App Design</t>
   </si>
   <si>
@@ -80,9 +78,6 @@
     <t>Tempo Control</t>
   </si>
   <si>
-    <t>Simple Audio Playback</t>
-  </si>
-  <si>
     <t>Design Planning</t>
   </si>
   <si>
@@ -96,12 +91,33 @@
   </si>
   <si>
     <t>Web App Music Writer</t>
+  </si>
+  <si>
+    <t>SOFTWARE</t>
+  </si>
+  <si>
+    <t>INTEGRATION</t>
+  </si>
+  <si>
+    <t>HARDWARE</t>
+  </si>
+  <si>
+    <t>Single Crotchet Playback</t>
+  </si>
+  <si>
+    <t>Multiple Octaves</t>
+  </si>
+  <si>
+    <t>Different Note Types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin Wave </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -119,7 +135,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -138,6 +154,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -151,13 +173,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,146 +501,217 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="4.21875" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="1" t="s">
+    <row r="2" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B13" s="7"/>
+      <c r="C13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B16" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+    </row>
+    <row r="17" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+    </row>
+    <row r="18" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+    </row>
+    <row r="19" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="4"/>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B3:C3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Presentation, fixed bug, and initial attempt at modifying the input format
Presentation, fixed bug, and initial attempt at modifying the input
format
</commit_message>
<xml_diff>
--- a/Presentations/Gantt Chart.xlsx
+++ b/Presentations/Gantt Chart.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27510"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\OneDrive - UNSW\Documents\2017 Semester 2\COMP3601 - Desgin Project A\Git Repositry\Presentations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isabelbarlow/MusicPlayer/Music-Player/Presentations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="C685E72BA27742A5988848DE9270A9F692B2FFBC" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21" xr10:uidLastSave="{C19839EE-7A0A-4BEC-B8E6-76B26FC5D67A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19368" windowHeight="10572" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Week 2</t>
   </si>
@@ -112,12 +117,15 @@
   </si>
   <si>
     <t xml:space="preserve">Sin Wave </t>
+  </si>
+  <si>
+    <t>Flash Memory</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -156,7 +164,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -183,10 +191,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -501,20 +509,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:O19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="4.21875" customWidth="1"/>
+    <col min="2" max="2" width="4.1640625" customWidth="1"/>
     <col min="3" max="3" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
@@ -552,21 +560,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="6" t="s">
+    <row r="3" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="6"/>
+      <c r="C3" s="8"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="6" t="s">
+    <row r="4" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="8"/>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C4" s="8"/>
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
@@ -574,12 +582,12 @@
       <c r="F5" s="3"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
-      <c r="I5" s="4"/>
+      <c r="I5" s="9"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
@@ -588,19 +596,19 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C7" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="4"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="9"/>
       <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
@@ -609,22 +617,22 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B9" s="6" t="s">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B9" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="6"/>
+      <c r="C9" s="8"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C10" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C11" s="1" t="s">
         <v>26</v>
       </c>
@@ -633,9 +641,9 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B12" s="7"/>
-      <c r="C12" s="7" t="s">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B12" s="6"/>
+      <c r="C12" s="6" t="s">
         <v>27</v>
       </c>
       <c r="E12" s="5"/>
@@ -643,8 +651,8 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B13" s="7"/>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B13" s="6"/>
       <c r="C13" s="1" t="s">
         <v>16</v>
       </c>
@@ -653,61 +661,69 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C14" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
-      <c r="I14" s="4"/>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="I14" s="9"/>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
-      <c r="I15" s="4"/>
+      <c r="I15" s="9"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B16" s="6" t="s">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I16" s="9"/>
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B17" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-    </row>
-    <row r="17" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="8"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-    </row>
-    <row r="18" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C18" s="1" t="s">
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-    </row>
-    <row r="19" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C19" s="1" t="s">
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B3:C3"/>

</xml_diff>

<commit_message>
Addeded rests and BMP to website
</commit_message>
<xml_diff>
--- a/Presentations/Gantt Chart.xlsx
+++ b/Presentations/Gantt Chart.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27510"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isabelbarlow/MusicPlayer/Music-Player/Presentations/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\OneDrive - UNSW\Documents\2017 Semester 2\COMP3601 - Desgin Project A\Git Repositry\Presentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="41" documentId="D04D10913DF381B9A04D5F42A7ACB6F80F3859BE" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{F27141D5-3E7B-4271-8422-6D40D80BF686}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="15996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,18 +20,18 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Week 2</t>
   </si>
@@ -120,13 +121,16 @@
   </si>
   <si>
     <t>Flash Memory</t>
+  </si>
+  <si>
+    <t>Week 13</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,8 +146,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -159,12 +170,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -184,18 +189,18 @@
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,20 +514,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:O20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="4.1640625" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" style="5"/>
+    <col min="2" max="2" width="4.109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" style="5" customWidth="1"/>
+    <col min="4" max="16384" width="8.77734375" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
@@ -559,167 +566,199 @@
       <c r="O2" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="8" t="s">
+      <c r="P2" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="8" t="s">
+      <c r="C3" s="2"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="7"/>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C4" s="2"/>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="8"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="M6" s="6"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="7"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B9" s="8" t="s">
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="8"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C9" s="2"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="E10" s="6"/>
+      <c r="F10" s="7"/>
+      <c r="L10" s="6"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B12" s="6"/>
-      <c r="C12" s="6" t="s">
+      <c r="E11" s="7"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="L11" s="6"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B12" s="9"/>
+      <c r="C12" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B13" s="6"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="L12" s="6"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B13" s="9"/>
       <c r="C13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="4"/>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="8"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I16" s="9"/>
-      <c r="J16" s="4"/>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B17" s="8" t="s">
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B17" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-    </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C17" s="2"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>